<commit_message>
Add more test clusters , add more stemming and normalizing rules to Continuous testing script.
</commit_message>
<xml_diff>
--- a/stemming_rules.xlsx
+++ b/stemming_rules.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
   <si>
     <t>from_suffix</t>
   </si>
@@ -38,7 +38,7 @@
     <t>ye,e,e+y,aye</t>
   </si>
   <si>
-    <t>(kamine , kamine+y , kaminye -&gt; kamina ; gaye -&gt; gaya ; apne -&gt; apna)</t>
+    <t>(kamine , kamine+y , kaminye -&gt; kamina ; gaye -&gt; gaya ; apne -&gt; apna) X hadapne , hadapna -&gt; hadap</t>
   </si>
   <si>
     <t>u</t>
@@ -71,7 +71,7 @@
     <t>(bajao -&gt; baja)</t>
   </si>
   <si>
-    <t>(dij)?ie     ,       (dij)?iey   ,     (dij)?iye   ,    (dij)?iy[ie]?(h+)?    ,    (dij)?i[ie]?y(h+)?</t>
+    <t>a?(dij)?ie     ,       a?(dij)?iey   ,     a?(dij)?iye   ,    a?(dij)?iy[ie]?(h+)?    ,    a?(dij)?i[ie]?y(h+)?</t>
   </si>
   <si>
     <t>(bata{dij}ie , bata{dij}iey , bata{dij}iye , bata{dij}iyeh -&gt; bata)</t>
@@ -95,10 +95,16 @@
     <t>ni,nee</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>te,tey</t>
+    <t>ana</t>
+  </si>
+  <si>
+    <t>(batana -&gt; bata ; katvana -&gt; katva)</t>
+  </si>
+  <si>
+    <t>te+i?(n)? ,te+y</t>
+  </si>
+  <si>
+    <t>(batate , batatein , batatey -&gt; bata )</t>
   </si>
   <si>
     <t>in,ing</t>
@@ -152,9 +158,6 @@
     <t>ane,aney,anay</t>
   </si>
   <si>
-    <t>ana</t>
-  </si>
-  <si>
     <t>ate,atey,ate</t>
   </si>
   <si>
@@ -194,16 +197,16 @@
     <t>aoge,aoge,aogey</t>
   </si>
   <si>
-    <t>engi,engee</t>
-  </si>
-  <si>
-    <t>enge,engey</t>
-  </si>
-  <si>
-    <t>ungi,ungee,oongi,oongee</t>
-  </si>
-  <si>
-    <t>unga,oonga</t>
+    <t>en?gi,en?ge+</t>
+  </si>
+  <si>
+    <t>en?ge,enge+y,en?ga</t>
+  </si>
+  <si>
+    <t>un?g(i+|e+)</t>
+  </si>
+  <si>
+    <t>un?ga,o+n?ga</t>
   </si>
   <si>
     <t>atin</t>
@@ -221,13 +224,28 @@
     <t>taen,taey,taye</t>
   </si>
   <si>
+    <t>iya+n,iya+</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>(kamzoriyaan , kamzoriya -&gt; kamzori)</t>
+  </si>
+  <si>
+    <t>iyon,iyo,io</t>
+  </si>
+  <si>
+    <t>(kamzoriyon , kamzoriyo , kamzorio-&gt; kamzori)</t>
+  </si>
+  <si>
     <t>iyan,iya</t>
   </si>
   <si>
-    <t>iyon,iyo</t>
-  </si>
-  <si>
-    <t>aengi,aengee</t>
+    <t>e(n)?gi,e(n)?gyi?</t>
+  </si>
+  <si>
+    <t>Laegi , laengi , laengee , laengy , laengi , laengyi-&gt; la</t>
   </si>
   <si>
     <t>e{n}ge,e{n}gey</t>
@@ -242,13 +260,55 @@
     <t>(banauangi , bataungi -&gt; bana , bata)</t>
   </si>
   <si>
-    <t>aunga, aoonga</t>
+    <t>aunga, ao+nga</t>
   </si>
   <si>
     <t>(banauanga , bataunga -&gt; bana , bata)</t>
   </si>
   <si>
     <t>ya</t>
+  </si>
+  <si>
+    <t>(a)+(u|o)n?gi,(a)+oon?gi,(a)+on?gee</t>
+  </si>
+  <si>
+    <t>(a)+(u|o)n?ga+,(a)+oon?ga+,(a)+on?ga+</t>
+  </si>
+  <si>
+    <t>(a)+(u|o)n?ge+y?</t>
+  </si>
+  <si>
+    <t>ha+n</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>beintahaan , beintaha -&gt; beintaha</t>
+  </si>
+  <si>
+    <t>khori</t>
+  </si>
+  <si>
+    <t>Haramkhori -&gt; haram</t>
+  </si>
+  <si>
+    <t>sh?a?li</t>
+  </si>
+  <si>
+    <t>vidyashali -&gt; vidya</t>
+  </si>
+  <si>
+    <t>van</t>
+  </si>
+  <si>
+    <t>vidyavan -&gt; vidya</t>
+  </si>
+  <si>
+    <t>ka?ra?n</t>
+  </si>
+  <si>
+    <t>abhivyaktikaran -&gt; abhivyakti</t>
   </si>
 </sst>
 </file>
@@ -345,10 +405,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A38" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A58" activeCellId="0" pane="topLeft" sqref="A58"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B66" activeCellId="0" pane="topLeft" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -441,7 +501,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>19</v>
@@ -490,20 +550,26 @@
         <v>26</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>9</v>
@@ -511,7 +577,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>9</v>
@@ -519,7 +585,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>9</v>
@@ -527,7 +593,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>9</v>
@@ -535,40 +601,40 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>4</v>
@@ -576,7 +642,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>9</v>
@@ -592,7 +658,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>9</v>
@@ -600,7 +666,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>9</v>
@@ -608,7 +674,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>9</v>
@@ -616,7 +682,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>9</v>
@@ -624,7 +690,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>9</v>
@@ -632,7 +698,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>9</v>
@@ -640,7 +706,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>9</v>
@@ -648,7 +714,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>9</v>
@@ -656,7 +722,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>9</v>
@@ -664,7 +730,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>9</v>
@@ -672,7 +738,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>9</v>
@@ -680,7 +746,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>9</v>
@@ -688,7 +754,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>9</v>
@@ -696,7 +762,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>9</v>
@@ -704,7 +770,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>9</v>
@@ -712,7 +778,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>9</v>
@@ -720,7 +786,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>9</v>
@@ -728,7 +794,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>4</v>
@@ -736,7 +802,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>9</v>
@@ -744,23 +810,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>4</v>
@@ -768,15 +834,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>9</v>
@@ -784,7 +850,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>9</v>
@@ -792,7 +858,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>9</v>
@@ -800,7 +866,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>9</v>
@@ -808,7 +874,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>9</v>
@@ -816,75 +882,163 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>9</v>
+        <v>70</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="A61" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="A62" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
+      <c r="A63" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
+      <c r="A64" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+      <c r="A65" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
+      <c r="A66" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="67">
+      <c r="A67" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
+      <c r="A68" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update more stemming and normalizing more rule, and improve the continuous tester script.
</commit_message>
<xml_diff>
--- a/stemming_rules.xlsx
+++ b/stemming_rules.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
   <si>
     <t>from_suffix</t>
   </si>
@@ -164,7 +164,13 @@
     <t>ati,atee</t>
   </si>
   <si>
-    <t>ata</t>
+    <t>(^\w.*?[^aeiou][ai]?)ta</t>
+  </si>
+  <si>
+    <t>\1</t>
+  </si>
+  <si>
+    <t>Adhunikata , adhunik  [Change only if it is preceded by 2 consonants(ie: syllables).... eg (bata !-&gt; ba ) X]  (visheshta -&gt; vishesh) , (pravahita -&gt; pravah)</t>
   </si>
   <si>
     <t>tin</t>
@@ -309,6 +315,30 @@
   </si>
   <si>
     <t>abhivyaktikaran -&gt; abhivyakti</t>
+  </si>
+  <si>
+    <t>wala</t>
+  </si>
+  <si>
+    <t>bichwala -&gt; bich</t>
+  </si>
+  <si>
+    <t>khani</t>
+  </si>
+  <si>
+    <t>Chedkhani -&gt; cheda</t>
+  </si>
+  <si>
+    <t>ma?nda?</t>
+  </si>
+  <si>
+    <t>Zaruratmand -&gt; zarurat</t>
+  </si>
+  <si>
+    <t>ika?</t>
+  </si>
+  <si>
+    <t>Itihasik -&gt; itihas</t>
   </si>
 </sst>
 </file>
@@ -383,8 +413,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -405,10 +439,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B66" activeCellId="0" pane="topLeft" sqref="B66"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A59" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A72" activeCellId="0" pane="topLeft" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -725,12 +759,15 @@
         <v>49</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>9</v>
@@ -738,7 +775,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>9</v>
@@ -746,7 +783,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>9</v>
@@ -754,7 +791,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>9</v>
@@ -762,7 +799,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>9</v>
@@ -770,7 +807,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>9</v>
@@ -778,7 +815,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>9</v>
@@ -786,7 +823,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>9</v>
@@ -794,7 +831,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>4</v>
@@ -802,7 +839,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>9</v>
@@ -810,7 +847,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>4</v>
@@ -818,7 +855,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>4</v>
@@ -826,7 +863,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>4</v>
@@ -834,7 +871,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>4</v>
@@ -842,7 +879,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>9</v>
@@ -850,7 +887,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>9</v>
@@ -858,7 +895,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>9</v>
@@ -866,7 +903,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>9</v>
@@ -874,7 +911,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>9</v>
@@ -882,29 +919,29 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>4</v>
@@ -912,51 +949,51 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>4</v>
@@ -964,7 +1001,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>4</v>
@@ -972,7 +1009,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>4</v>
@@ -980,7 +1017,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>4</v>
@@ -988,57 +1025,101 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
+      <c r="A69" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
+      <c r="A70" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="71">
+      <c r="A71" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="72">
+      <c r="A72" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>